<commit_message>
Updated Intro according to Alie's suggestions and her areas of expertise
</commit_message>
<xml_diff>
--- a/data/Info_on_people.xlsx
+++ b/data/Info_on_people.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Urs/ownCloud/MPI/Methods_Support_Program/methods_support_repository/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0179ECC1-B17F-7F45-B965-29058FCEB4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3286173B-2C8E-3245-963B-CFD68315EB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5500" yWindow="500" windowWidth="45700" windowHeight="26500" activeTab="3" xr2:uid="{06468B05-62F6-4C44-85A6-01C0375D22DD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26500" activeTab="2" xr2:uid="{06468B05-62F6-4C44-85A6-01C0375D22DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Name_table" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="137">
   <si>
     <t>Name</t>
   </si>
@@ -382,12 +382,6 @@
   </si>
   <si>
     <t>Data visualization (including mapping) (conceptualization +/ execution in R)</t>
-  </si>
-  <si>
-    <t>Basic frequentist stats (parametric and non-parametric)</t>
-  </si>
-  <si>
-    <t>General and generalized linear (mixed) modelling (GL(M)Ms and L(M)Ms)</t>
   </si>
   <si>
     <t>Basic movement analysis (calculating home ranges, DJLs, etc)</t>
@@ -559,11 +553,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -916,7 +910,7 @@
         <v>114</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>115</v>
@@ -927,7 +921,7 @@
         <v>93</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>102</v>
@@ -950,7 +944,7 @@
         <v>94</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>103</v>
@@ -973,7 +967,7 @@
         <v>95</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>104</v>
@@ -996,7 +990,7 @@
         <v>96</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>105</v>
@@ -1019,7 +1013,7 @@
         <v>97</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>106</v>
@@ -1034,7 +1028,7 @@
         <v>31</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1042,7 +1036,7 @@
         <v>98</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>107</v>
@@ -1065,7 +1059,7 @@
         <v>99</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>108</v>
@@ -1088,7 +1082,7 @@
         <v>100</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>109</v>
@@ -1111,7 +1105,7 @@
         <v>101</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>110</v>
@@ -1131,13 +1125,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D11" s="7">
         <v>2</v>
@@ -1151,7 +1145,7 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1552,13 +1546,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
         <v>132</v>
-      </c>
-      <c r="B1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" t="s">
-        <v>134</v>
       </c>
       <c r="D1" t="s">
         <v>90</v>
@@ -1568,10 +1562,10 @@
       <c r="A2">
         <v>39</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="17">
         <v>44466</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="17">
         <v>44470</v>
       </c>
       <c r="D2" s="10" t="s">
@@ -1582,10 +1576,10 @@
       <c r="A3">
         <v>39</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="17">
         <v>44466</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="17">
         <v>44470</v>
       </c>
       <c r="D3" s="10" t="s">
@@ -1596,10 +1590,10 @@
       <c r="A4">
         <v>40</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="17">
         <v>44473</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="17">
         <v>44477</v>
       </c>
       <c r="D4" s="10" t="s">
@@ -1610,10 +1604,10 @@
       <c r="A5">
         <v>40</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="17">
         <v>44473</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="17">
         <v>44477</v>
       </c>
       <c r="D5" s="10" t="s">
@@ -1624,10 +1618,10 @@
       <c r="A6">
         <v>41</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="17">
         <v>44480</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="17">
         <v>44484</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -1638,10 +1632,10 @@
       <c r="A7">
         <v>41</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="17">
         <v>44480</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="17">
         <v>44484</v>
       </c>
       <c r="D7" s="10" t="s">
@@ -1652,10 +1646,10 @@
       <c r="A8">
         <v>42</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="17">
         <v>44487</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="17">
         <v>44491</v>
       </c>
       <c r="D8" s="10" t="s">
@@ -1666,24 +1660,24 @@
       <c r="A9">
         <v>42</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="17">
         <v>44487</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="17">
         <v>44491</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>43</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="17">
         <v>44494</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="17">
         <v>44498</v>
       </c>
       <c r="D10" s="10" t="s">
@@ -1694,10 +1688,10 @@
       <c r="A11">
         <v>43</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="17">
         <v>44494</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="17">
         <v>44498</v>
       </c>
       <c r="D11" s="10" t="s">
@@ -1708,10 +1702,10 @@
       <c r="A12">
         <v>44</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="17">
         <v>44501</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="17">
         <v>44505</v>
       </c>
       <c r="D12" s="10" t="s">
@@ -1722,10 +1716,10 @@
       <c r="A13">
         <v>44</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="17">
         <v>44501</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="17">
         <v>44505</v>
       </c>
       <c r="D13" s="10" t="s">
@@ -1736,10 +1730,10 @@
       <c r="A14">
         <v>45</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="17">
         <v>44508</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="17">
         <v>44512</v>
       </c>
       <c r="D14" s="10" t="s">
@@ -1750,10 +1744,10 @@
       <c r="A15">
         <v>45</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="17">
         <v>44508</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="17">
         <v>44512</v>
       </c>
       <c r="D15" s="10" t="s">
@@ -1764,10 +1758,10 @@
       <c r="A16">
         <v>46</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="17">
         <v>44515</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="17">
         <v>44519</v>
       </c>
       <c r="D16" s="10" t="s">
@@ -1778,10 +1772,10 @@
       <c r="A17">
         <v>46</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="17">
         <v>44515</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="17">
         <v>44519</v>
       </c>
       <c r="D17" s="10" t="s">
@@ -1792,10 +1786,10 @@
       <c r="A18">
         <v>47</v>
       </c>
-      <c r="B18" s="21">
+      <c r="B18" s="17">
         <v>44522</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C18" s="17">
         <v>44526</v>
       </c>
       <c r="D18" s="10" t="s">
@@ -1806,24 +1800,24 @@
       <c r="A19">
         <v>47</v>
       </c>
-      <c r="B19" s="21">
+      <c r="B19" s="17">
         <v>44522</v>
       </c>
-      <c r="C19" s="21">
+      <c r="C19" s="17">
         <v>44526</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>48</v>
       </c>
-      <c r="B20" s="21">
+      <c r="B20" s="17">
         <v>44529</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C20" s="17">
         <v>44533</v>
       </c>
       <c r="D20" s="10" t="s">
@@ -1835,10 +1829,10 @@
       <c r="A21">
         <v>48</v>
       </c>
-      <c r="B21" s="21">
+      <c r="B21" s="17">
         <v>44529</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="17">
         <v>44533</v>
       </c>
       <c r="D21" s="10" t="s">
@@ -1849,10 +1843,10 @@
       <c r="A22">
         <v>49</v>
       </c>
-      <c r="B22" s="21">
+      <c r="B22" s="17">
         <v>44536</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="17">
         <v>44540</v>
       </c>
       <c r="D22" s="10" t="s">
@@ -1863,10 +1857,10 @@
       <c r="A23">
         <v>49</v>
       </c>
-      <c r="B23" s="21">
+      <c r="B23" s="17">
         <v>44536</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C23" s="17">
         <v>44540</v>
       </c>
       <c r="D23" s="10" t="s">
@@ -1877,10 +1871,10 @@
       <c r="A24">
         <v>50</v>
       </c>
-      <c r="B24" s="21">
+      <c r="B24" s="17">
         <v>44543</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="17">
         <v>44547</v>
       </c>
       <c r="D24" s="10" t="s">
@@ -1891,10 +1885,10 @@
       <c r="A25">
         <v>50</v>
       </c>
-      <c r="B25" s="21">
+      <c r="B25" s="17">
         <v>44543</v>
       </c>
-      <c r="C25" s="21">
+      <c r="C25" s="17">
         <v>44547</v>
       </c>
       <c r="D25" s="10" t="s">
@@ -1935,10 +1929,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15B9AB3-2715-044A-BA8C-589BC5134BD9}">
-  <dimension ref="A1:B79"/>
+  <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1951,7 +1945,7 @@
         <v>90</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1988,18 +1982,18 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>118</v>
+        <v>94</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>119</v>
+        <v>94</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -2007,7 +2001,7 @@
         <v>94</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2015,7 +2009,7 @@
         <v>94</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -2023,7 +2017,7 @@
         <v>94</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -2031,7 +2025,7 @@
         <v>94</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -2039,7 +2033,7 @@
         <v>94</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -2047,7 +2041,7 @@
         <v>94</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -2055,7 +2049,7 @@
         <v>94</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -2063,23 +2057,23 @@
         <v>94</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -2087,7 +2081,7 @@
         <v>95</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -2095,7 +2089,7 @@
         <v>95</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -2103,23 +2097,23 @@
         <v>95</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -2127,7 +2121,7 @@
         <v>96</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -2135,7 +2129,7 @@
         <v>96</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -2143,23 +2137,23 @@
         <v>96</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -2167,7 +2161,7 @@
         <v>97</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -2175,7 +2169,7 @@
         <v>97</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -2183,7 +2177,7 @@
         <v>97</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -2191,7 +2185,7 @@
         <v>97</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -2199,7 +2193,7 @@
         <v>97</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -2207,23 +2201,23 @@
         <v>97</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>46</v>
+        <v>98</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>47</v>
+        <v>98</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -2231,7 +2225,7 @@
         <v>98</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -2239,7 +2233,7 @@
         <v>98</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -2247,7 +2241,7 @@
         <v>98</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -2255,23 +2249,23 @@
         <v>98</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -2279,7 +2273,7 @@
         <v>99</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -2287,7 +2281,7 @@
         <v>99</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -2295,7 +2289,7 @@
         <v>99</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -2303,23 +2297,23 @@
         <v>99</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>62</v>
+        <v>100</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>63</v>
+        <v>100</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -2327,7 +2321,7 @@
         <v>100</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -2335,7 +2329,7 @@
         <v>100</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -2343,7 +2337,7 @@
         <v>100</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -2351,7 +2345,7 @@
         <v>100</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -2359,7 +2353,7 @@
         <v>100</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -2367,7 +2361,7 @@
         <v>100</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -2375,7 +2369,7 @@
         <v>100</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -2383,7 +2377,7 @@
         <v>100</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -2391,7 +2385,7 @@
         <v>100</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -2399,7 +2393,7 @@
         <v>100</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -2407,7 +2401,7 @@
         <v>100</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -2415,7 +2409,7 @@
         <v>100</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -2423,23 +2417,23 @@
         <v>100</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>79</v>
+        <v>101</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>80</v>
+        <v>101</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -2447,7 +2441,7 @@
         <v>101</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -2455,7 +2449,7 @@
         <v>101</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -2463,7 +2457,7 @@
         <v>101</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -2471,7 +2465,7 @@
         <v>101</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -2479,7 +2473,7 @@
         <v>101</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -2487,7 +2481,7 @@
         <v>101</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -2495,28 +2489,28 @@
         <v>101</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>87</v>
+        <v>128</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>88</v>
+        <v>128</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>120</v>
@@ -2524,7 +2518,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>121</v>
@@ -2532,7 +2526,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>122</v>
@@ -2540,7 +2534,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>123</v>
@@ -2548,7 +2542,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>124</v>
@@ -2556,26 +2550,10 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2587,7 +2565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CAEC49A-A771-EC43-9543-B7500F1AD0CA}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="P44" sqref="P44"/>
     </sheetView>
   </sheetViews>
@@ -2611,291 +2589,291 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>102</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="18"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="19"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="18" t="s">
         <v>103</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="18" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="17"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="18" t="s">
         <v>104</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="18" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="17"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="17"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="17"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="17"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="18" t="s">
         <v>105</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="18" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="17"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="17"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="17"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="17"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="18" t="s">
         <v>106</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="D29" s="18" t="s">
         <v>31</v>
       </c>
       <c r="E29" s="20" t="s">
@@ -2903,506 +2881,530 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="17"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
       <c r="E30" s="20"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="17"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
       <c r="E31" s="20"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="17"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
       <c r="E32" s="20"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="17"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
       <c r="E33" s="20"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="17"/>
+      <c r="A34" s="18"/>
       <c r="B34" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
       <c r="E34" s="20"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="17"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
       <c r="E35" s="20"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="17"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
       <c r="E36" s="20"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="17" t="s">
-        <v>138</v>
+      <c r="A37" s="18" t="s">
+        <v>136</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="C37" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D37" s="18" t="s">
+      <c r="D37" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="18" t="s">
+      <c r="E37" s="19" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="17"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="17"/>
+      <c r="A39" s="18"/>
       <c r="B39" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="17"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="17"/>
+      <c r="A41" s="18"/>
       <c r="B41" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="17"/>
+      <c r="A42" s="18"/>
       <c r="B42" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="18" t="s">
         <v>108</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C43" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="18" t="s">
+      <c r="D43" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E43" s="18" t="s">
+      <c r="E43" s="19" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="17"/>
+      <c r="A44" s="18"/>
       <c r="B44" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="17"/>
+      <c r="A45" s="18"/>
       <c r="B45" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="17"/>
+      <c r="A46" s="18"/>
       <c r="B46" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="17"/>
+      <c r="A47" s="18"/>
       <c r="B47" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="17"/>
+      <c r="A48" s="18"/>
       <c r="B48" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="19" t="s">
+      <c r="A49" s="21" t="s">
         <v>109</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C49" s="19" t="s">
+      <c r="C49" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D49" s="18" t="s">
+      <c r="D49" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="E49" s="18" t="s">
+      <c r="E49" s="19" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="19"/>
+      <c r="A50" s="21"/>
       <c r="B50" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C50" s="19"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="19"/>
+      <c r="A51" s="21"/>
       <c r="B51" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C51" s="19"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="19"/>
+      <c r="A52" s="21"/>
       <c r="B52" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C52" s="19"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="19"/>
+      <c r="A53" s="21"/>
       <c r="B53" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C53" s="19"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="19"/>
+      <c r="A54" s="21"/>
       <c r="B54" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C54" s="19"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="19"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C55" s="19"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="19"/>
+      <c r="A56" s="21"/>
       <c r="B56" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C56" s="19"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="19"/>
+      <c r="A57" s="21"/>
       <c r="B57" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C57" s="19"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="19"/>
+      <c r="A58" s="21"/>
       <c r="B58" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C58" s="19"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="19"/>
+      <c r="A59" s="21"/>
       <c r="B59" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C59" s="19"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="18"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="19"/>
+      <c r="A60" s="21"/>
       <c r="B60" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C60" s="19"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="19"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C61" s="19"/>
-      <c r="D61" s="18"/>
-      <c r="E61" s="18"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="19"/>
+      <c r="A62" s="21"/>
       <c r="B62" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C62" s="19"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="19"/>
+      <c r="A63" s="21"/>
       <c r="B63" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C63" s="19"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="17" t="s">
+      <c r="A64" s="18" t="s">
         <v>110</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C64" s="17" t="s">
+      <c r="C64" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D64" s="18" t="s">
+      <c r="D64" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E64" s="18" t="s">
+      <c r="E64" s="19" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="17"/>
+      <c r="A65" s="18"/>
       <c r="B65" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C65" s="17"/>
-      <c r="D65" s="18"/>
-      <c r="E65" s="18"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="17"/>
+      <c r="A66" s="18"/>
       <c r="B66" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C66" s="17"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="17"/>
+      <c r="A67" s="18"/>
       <c r="B67" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C67" s="17"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="18"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="19"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="17"/>
+      <c r="A68" s="18"/>
       <c r="B68" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C68" s="17"/>
-      <c r="D68" s="18"/>
-      <c r="E68" s="18"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="19"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="17"/>
+      <c r="A69" s="18"/>
       <c r="B69" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C69" s="17"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="18"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="17"/>
+      <c r="A70" s="18"/>
       <c r="B70" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C70" s="17"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="18"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="17"/>
+      <c r="A71" s="18"/>
       <c r="B71" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C71" s="17"/>
-      <c r="D71" s="18"/>
-      <c r="E71" s="18"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="17"/>
+      <c r="A72" s="18"/>
       <c r="B72" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C72" s="17"/>
-      <c r="D72" s="18"/>
-      <c r="E72" s="18"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="17" t="s">
-        <v>129</v>
+      <c r="A73" s="18" t="s">
+        <v>127</v>
       </c>
       <c r="B73" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C73" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D73" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E73" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="18"/>
+      <c r="B74" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="19"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="18"/>
+      <c r="B75" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C73" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D73" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E73" s="18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="17"/>
-      <c r="B74" s="6" t="s">
+      <c r="C75" s="19"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="19"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="18"/>
+      <c r="B76" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C74" s="18"/>
-      <c r="D74" s="18"/>
-      <c r="E74" s="18"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="17"/>
-      <c r="B75" s="6" t="s">
+      <c r="C76" s="19"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="19"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="18"/>
+      <c r="B77" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C75" s="18"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="18"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" s="17"/>
-      <c r="B76" s="6" t="s">
+      <c r="C77" s="19"/>
+      <c r="D77" s="19"/>
+      <c r="E77" s="19"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="18"/>
+      <c r="B78" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C76" s="18"/>
-      <c r="D76" s="18"/>
-      <c r="E76" s="18"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="17"/>
-      <c r="B77" s="6" t="s">
+      <c r="C78" s="19"/>
+      <c r="D78" s="19"/>
+      <c r="E78" s="19"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="18"/>
+      <c r="B79" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C77" s="18"/>
-      <c r="D77" s="18"/>
-      <c r="E77" s="18"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" s="17"/>
-      <c r="B78" s="6" t="s">
+      <c r="C79" s="19"/>
+      <c r="D79" s="19"/>
+      <c r="E79" s="19"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="18"/>
+      <c r="B80" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C78" s="18"/>
-      <c r="D78" s="18"/>
-      <c r="E78" s="18"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" s="17"/>
-      <c r="B79" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C79" s="18"/>
-      <c r="D79" s="18"/>
-      <c r="E79" s="18"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" s="17"/>
-      <c r="B80" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C80" s="18"/>
-      <c r="D80" s="18"/>
-      <c r="E80" s="18"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="D37:D42"/>
+    <mergeCell ref="E37:E42"/>
+    <mergeCell ref="A64:A72"/>
+    <mergeCell ref="C64:C72"/>
+    <mergeCell ref="D64:D72"/>
+    <mergeCell ref="E64:E72"/>
+    <mergeCell ref="A43:A48"/>
+    <mergeCell ref="C43:C48"/>
+    <mergeCell ref="D43:D48"/>
+    <mergeCell ref="E43:E48"/>
+    <mergeCell ref="A49:A63"/>
+    <mergeCell ref="C49:C63"/>
+    <mergeCell ref="D49:D63"/>
+    <mergeCell ref="E49:E63"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="D24:D28"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="A29:A36"/>
+    <mergeCell ref="C29:C36"/>
+    <mergeCell ref="D29:D36"/>
+    <mergeCell ref="E29:E36"/>
     <mergeCell ref="A73:A80"/>
     <mergeCell ref="C73:C80"/>
     <mergeCell ref="D73:D80"/>
@@ -3419,30 +3421,6 @@
     <mergeCell ref="C19:C23"/>
     <mergeCell ref="D19:D23"/>
     <mergeCell ref="E19:E23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="C24:C28"/>
-    <mergeCell ref="D24:D28"/>
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="A29:A36"/>
-    <mergeCell ref="C29:C36"/>
-    <mergeCell ref="D29:D36"/>
-    <mergeCell ref="E29:E36"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="C37:C42"/>
-    <mergeCell ref="D37:D42"/>
-    <mergeCell ref="E37:E42"/>
-    <mergeCell ref="A64:A72"/>
-    <mergeCell ref="C64:C72"/>
-    <mergeCell ref="D64:D72"/>
-    <mergeCell ref="E64:E72"/>
-    <mergeCell ref="A43:A48"/>
-    <mergeCell ref="C43:C48"/>
-    <mergeCell ref="D43:D48"/>
-    <mergeCell ref="E43:E48"/>
-    <mergeCell ref="A49:A63"/>
-    <mergeCell ref="C49:C63"/>
-    <mergeCell ref="D49:D63"/>
-    <mergeCell ref="E49:E63"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E29" r:id="rId1" display="mailto:estrauss@ab.mpg.de" xr:uid="{4578C63B-D32E-F34D-83CB-32A0DE28B1B1}"/>

</xml_diff>

<commit_message>
Included current schedule on intro page, added info on people
</commit_message>
<xml_diff>
--- a/data/Info_on_people.xlsx
+++ b/data/Info_on_people.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Urs/ownCloud/MPI/Methods_Support_Program/methods_support_repository/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/urskalbitzer/ownCloud/MPI/Methods_Support_Program/methods_support_repository/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3286173B-2C8E-3245-963B-CFD68315EB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E96B0AD-3ADF-5142-93C0-1612CACCA8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26500" activeTab="2" xr2:uid="{06468B05-62F6-4C44-85A6-01C0375D22DD}"/>
+    <workbookView xWindow="16800" yWindow="500" windowWidth="16800" windowHeight="20500" activeTab="2" xr2:uid="{06468B05-62F6-4C44-85A6-01C0375D22DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Name_table" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="139">
   <si>
     <t>Name</t>
   </si>
@@ -442,6 +442,12 @@
   </si>
   <si>
     <t>Vivek</t>
+  </si>
+  <si>
+    <t>eObs collars</t>
+  </si>
+  <si>
+    <t>endocrinology</t>
   </si>
 </sst>
 </file>
@@ -535,7 +541,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -555,9 +561,10 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1929,10 +1936,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15B9AB3-2715-044A-BA8C-589BC5134BD9}">
-  <dimension ref="A1:B77"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2142,18 +2149,18 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>40</v>
+        <v>96</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>41</v>
+        <v>96</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -2161,7 +2168,7 @@
         <v>97</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -2169,7 +2176,7 @@
         <v>97</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -2177,7 +2184,7 @@
         <v>97</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -2185,7 +2192,7 @@
         <v>97</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -2193,7 +2200,7 @@
         <v>97</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -2201,23 +2208,23 @@
         <v>97</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>50</v>
+        <v>97</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>51</v>
+        <v>97</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -2225,7 +2232,7 @@
         <v>98</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -2233,7 +2240,7 @@
         <v>98</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -2241,7 +2248,7 @@
         <v>98</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -2249,23 +2256,23 @@
         <v>98</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -2273,7 +2280,7 @@
         <v>99</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -2281,7 +2288,7 @@
         <v>99</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -2289,7 +2296,7 @@
         <v>99</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -2297,23 +2304,23 @@
         <v>99</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>66</v>
+        <v>99</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>67</v>
+        <v>99</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -2321,7 +2328,7 @@
         <v>100</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -2329,7 +2336,7 @@
         <v>100</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -2337,7 +2344,7 @@
         <v>100</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -2345,7 +2352,7 @@
         <v>100</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -2353,7 +2360,7 @@
         <v>100</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -2361,7 +2368,7 @@
         <v>100</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -2369,7 +2376,7 @@
         <v>100</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -2377,7 +2384,7 @@
         <v>100</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -2385,7 +2392,7 @@
         <v>100</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -2393,7 +2400,7 @@
         <v>100</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -2401,7 +2408,7 @@
         <v>100</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -2409,7 +2416,7 @@
         <v>100</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -2417,23 +2424,23 @@
         <v>100</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>40</v>
+        <v>100</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>83</v>
+        <v>100</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -2441,7 +2448,7 @@
         <v>101</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -2449,7 +2456,7 @@
         <v>101</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -2457,7 +2464,7 @@
         <v>101</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>84</v>
+        <v>42</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -2465,7 +2472,7 @@
         <v>101</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -2473,7 +2480,7 @@
         <v>101</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -2481,7 +2488,7 @@
         <v>101</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -2489,23 +2496,23 @@
         <v>101</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>118</v>
+        <v>101</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>119</v>
+        <v>101</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -2513,7 +2520,7 @@
         <v>128</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -2521,7 +2528,7 @@
         <v>128</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -2529,7 +2536,7 @@
         <v>128</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -2537,7 +2544,7 @@
         <v>128</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -2545,7 +2552,7 @@
         <v>128</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -2553,6 +2560,22 @@
         <v>128</v>
       </c>
       <c r="B77" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B79" s="6" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2589,483 +2612,483 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>102</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="20" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="20"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="19" t="s">
         <v>103</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="19" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="18"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="18"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="19" t="s">
         <v>104</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="19" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="18"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="18"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="19" t="s">
         <v>105</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="19" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="18"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="18"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="18"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="18"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="19" t="s">
         <v>106</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E29" s="22" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="18"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="20"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="22"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="18"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="20"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="22"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="18"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="20"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="22"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="18"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="20"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="22"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="18"/>
+      <c r="A34" s="19"/>
       <c r="B34" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="20"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="22"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="18"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="20"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="22"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="18"/>
+      <c r="A36" s="19"/>
       <c r="B36" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="20"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="22"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="19" t="s">
         <v>136</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="20" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="18"/>
+      <c r="A38" s="19"/>
       <c r="B38" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="18"/>
+      <c r="A39" s="19"/>
       <c r="B39" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="18"/>
+      <c r="A40" s="19"/>
       <c r="B40" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="18"/>
+      <c r="A41" s="19"/>
       <c r="B41" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="18"/>
+      <c r="A42" s="19"/>
       <c r="B42" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="19" t="s">
         <v>108</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C43" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="19" t="s">
+      <c r="D43" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E43" s="19" t="s">
+      <c r="E43" s="20" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="18"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="18"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="18"/>
+      <c r="A46" s="19"/>
       <c r="B46" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="18"/>
+      <c r="A47" s="19"/>
       <c r="B47" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="18"/>
+      <c r="A48" s="19"/>
       <c r="B48" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="21" t="s">
@@ -3077,10 +3100,10 @@
       <c r="C49" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D49" s="19" t="s">
+      <c r="D49" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="E49" s="19" t="s">
+      <c r="E49" s="20" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3090,8 +3113,8 @@
         <v>67</v>
       </c>
       <c r="C50" s="21"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="21"/>
@@ -3099,8 +3122,8 @@
         <v>68</v>
       </c>
       <c r="C51" s="21"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="21"/>
@@ -3108,8 +3131,8 @@
         <v>69</v>
       </c>
       <c r="C52" s="21"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="21"/>
@@ -3117,8 +3140,8 @@
         <v>70</v>
       </c>
       <c r="C53" s="21"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="21"/>
@@ -3126,8 +3149,8 @@
         <v>71</v>
       </c>
       <c r="C54" s="21"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="21"/>
@@ -3135,8 +3158,8 @@
         <v>72</v>
       </c>
       <c r="C55" s="21"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="21"/>
@@ -3144,8 +3167,8 @@
         <v>73</v>
       </c>
       <c r="C56" s="21"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="21"/>
@@ -3153,8 +3176,8 @@
         <v>74</v>
       </c>
       <c r="C57" s="21"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="21"/>
@@ -3162,8 +3185,8 @@
         <v>75</v>
       </c>
       <c r="C58" s="21"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="21"/>
@@ -3171,8 +3194,8 @@
         <v>76</v>
       </c>
       <c r="C59" s="21"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="19"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="21"/>
@@ -3180,8 +3203,8 @@
         <v>77</v>
       </c>
       <c r="C60" s="21"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="21"/>
@@ -3189,8 +3212,8 @@
         <v>78</v>
       </c>
       <c r="C61" s="21"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="19"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="21"/>
@@ -3198,8 +3221,8 @@
         <v>79</v>
       </c>
       <c r="C62" s="21"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="21"/>
@@ -3207,180 +3230,204 @@
         <v>80</v>
       </c>
       <c r="C63" s="21"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="19"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="20"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="18" t="s">
+      <c r="A64" s="19" t="s">
         <v>110</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C64" s="18" t="s">
+      <c r="C64" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D64" s="19" t="s">
+      <c r="D64" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E64" s="19" t="s">
+      <c r="E64" s="20" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="18"/>
+      <c r="A65" s="19"/>
       <c r="B65" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C65" s="18"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="19"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="20"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="18"/>
+      <c r="A66" s="19"/>
       <c r="B66" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C66" s="18"/>
-      <c r="D66" s="19"/>
-      <c r="E66" s="19"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="20"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="18"/>
+      <c r="A67" s="19"/>
       <c r="B67" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C67" s="18"/>
-      <c r="D67" s="19"/>
-      <c r="E67" s="19"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="20"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="18"/>
+      <c r="A68" s="19"/>
       <c r="B68" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C68" s="18"/>
-      <c r="D68" s="19"/>
-      <c r="E68" s="19"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="20"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="18"/>
+      <c r="A69" s="19"/>
       <c r="B69" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C69" s="18"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="20"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="18"/>
+      <c r="A70" s="19"/>
       <c r="B70" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C70" s="18"/>
-      <c r="D70" s="19"/>
-      <c r="E70" s="19"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="18"/>
+      <c r="A71" s="19"/>
       <c r="B71" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C71" s="18"/>
-      <c r="D71" s="19"/>
-      <c r="E71" s="19"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="20"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="18"/>
+      <c r="A72" s="19"/>
       <c r="B72" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C72" s="18"/>
-      <c r="D72" s="19"/>
-      <c r="E72" s="19"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="20"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="18" t="s">
+      <c r="A73" s="19" t="s">
         <v>127</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C73" s="19" t="s">
+      <c r="C73" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D73" s="19" t="s">
+      <c r="D73" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E73" s="19" t="s">
+      <c r="E73" s="20" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="18"/>
+      <c r="A74" s="19"/>
       <c r="B74" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C74" s="19"/>
-      <c r="D74" s="19"/>
-      <c r="E74" s="19"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="20"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="18"/>
+      <c r="A75" s="19"/>
       <c r="B75" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C75" s="19"/>
-      <c r="D75" s="19"/>
-      <c r="E75" s="19"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="20"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" s="18"/>
+      <c r="A76" s="19"/>
       <c r="B76" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C76" s="19"/>
-      <c r="D76" s="19"/>
-      <c r="E76" s="19"/>
+      <c r="C76" s="20"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="20"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="18"/>
+      <c r="A77" s="19"/>
       <c r="B77" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C77" s="19"/>
-      <c r="D77" s="19"/>
-      <c r="E77" s="19"/>
+      <c r="C77" s="20"/>
+      <c r="D77" s="20"/>
+      <c r="E77" s="20"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" s="18"/>
+      <c r="A78" s="19"/>
       <c r="B78" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C78" s="19"/>
-      <c r="D78" s="19"/>
-      <c r="E78" s="19"/>
+      <c r="C78" s="20"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="20"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" s="18"/>
+      <c r="A79" s="19"/>
       <c r="B79" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C79" s="19"/>
-      <c r="D79" s="19"/>
-      <c r="E79" s="19"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="20"/>
+      <c r="E79" s="20"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" s="18"/>
+      <c r="A80" s="19"/>
       <c r="B80" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C80" s="19"/>
-      <c r="D80" s="19"/>
-      <c r="E80" s="19"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A73:A80"/>
+    <mergeCell ref="C73:C80"/>
+    <mergeCell ref="D73:D80"/>
+    <mergeCell ref="E73:E80"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="E2:E8"/>
+    <mergeCell ref="A9:A18"/>
+    <mergeCell ref="C9:C18"/>
+    <mergeCell ref="D9:D18"/>
+    <mergeCell ref="E9:E18"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="D19:D23"/>
+    <mergeCell ref="E19:E23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="D24:D28"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="A29:A36"/>
+    <mergeCell ref="C29:C36"/>
+    <mergeCell ref="D29:D36"/>
+    <mergeCell ref="E29:E36"/>
     <mergeCell ref="A37:A42"/>
     <mergeCell ref="C37:C42"/>
     <mergeCell ref="D37:D42"/>
@@ -3397,30 +3444,6 @@
     <mergeCell ref="C49:C63"/>
     <mergeCell ref="D49:D63"/>
     <mergeCell ref="E49:E63"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="C24:C28"/>
-    <mergeCell ref="D24:D28"/>
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="A29:A36"/>
-    <mergeCell ref="C29:C36"/>
-    <mergeCell ref="D29:D36"/>
-    <mergeCell ref="E29:E36"/>
-    <mergeCell ref="A73:A80"/>
-    <mergeCell ref="C73:C80"/>
-    <mergeCell ref="D73:D80"/>
-    <mergeCell ref="E73:E80"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="C2:C8"/>
-    <mergeCell ref="D2:D8"/>
-    <mergeCell ref="E2:E8"/>
-    <mergeCell ref="A9:A18"/>
-    <mergeCell ref="C9:C18"/>
-    <mergeCell ref="D9:D18"/>
-    <mergeCell ref="E9:E18"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="D19:D23"/>
-    <mergeCell ref="E19:E23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E29" r:id="rId1" display="mailto:estrauss@ab.mpg.de" xr:uid="{4578C63B-D32E-F34D-83CB-32A0DE28B1B1}"/>

</xml_diff>